<commit_message>
estimated the copying cost CCSU copy center
 via Neva working with their website
</commit_message>
<xml_diff>
--- a/CookingWithComputingBudget.xlsx
+++ b/CookingWithComputingBudget.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Budget for dinner event</t>
   </si>
@@ -45,6 +45,33 @@
   </si>
   <si>
     <t>make sure the room seats this many</t>
+  </si>
+  <si>
+    <t>150 copies after we have the art, by CCSU Copy Center</t>
+  </si>
+  <si>
+    <t>the art: photography costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the recipes: </t>
+  </si>
+  <si>
+    <t>4 hours of the site</t>
+  </si>
+  <si>
+    <t>insurance: self insured</t>
+  </si>
+  <si>
+    <t>security:</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>people</t>
+  </si>
+  <si>
+    <t>per seat</t>
   </si>
 </sst>
 </file>
@@ -359,41 +386,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>150</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18">
+        <f>A18*C18</f>
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more budget estimation, routing sheet
</commit_message>
<xml_diff>
--- a/CookingWithComputingBudget.xlsx
+++ b/CookingWithComputingBudget.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24620" yWindow="2980" windowWidth="15380" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="24600" yWindow="2980" windowWidth="15380" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Budget for dinner event</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Recurring</t>
+  </si>
+  <si>
+    <t>first time direct cost</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -425,16 +428,25 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="F6">
+        <v>500</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
+      <c r="F8">
+        <v>500</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -453,6 +465,9 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -461,6 +476,9 @@
       <c r="B13" t="s">
         <v>12</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -501,7 +519,7 @@
       </c>
       <c r="H26">
         <f>F6+F7+F8</f>
-        <v>0</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -509,8 +527,17 @@
         <v>17</v>
       </c>
       <c r="H28">
-        <f>F5+F11+F19</f>
+        <f>F5+F11+F12+F13+F19</f>
         <v>5250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31">
+        <f>H26+H28</f>
+        <v>6280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>